<commit_message>
Ich habe die EchoPlay Chip Ersatz Planung fertiggestellt und habe an der Dokumentation geschrieben
</commit_message>
<xml_diff>
--- a/docs/250326_Materialliste EchoPlay_Tom_Nielsen.xlsx
+++ b/docs/250326_Materialliste EchoPlay_Tom_Nielsen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/tom_nielsen_edu_gbssg_ch/Documents/Schule/IMS/IP/LED-Box/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomni\Documents\Schule-lokal\IMS\IP\ims.project.echoplay\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="11_AD4DB114E441178AC67DF4D56611FE52683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53E48863-14D3-4C9B-AE6A-627076E29B51}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A2A949-181A-48D4-9CA6-9243BBB6F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>

</xml_diff>